<commit_message>
solved error in logic for the functions
</commit_message>
<xml_diff>
--- a/Casos de Prueba.xlsx
+++ b/Casos de Prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinil\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinil\Desktop\Universidad\Semestre 3\Codigo Limpio\Proyecto de aula\Icetex_Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1373919-3600-4607-85AF-A6DA57FCD65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9B41D-4B31-4BB6-84BE-D7B77C413DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -177,21 +177,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -583,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,48 +579,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -644,79 +665,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1016,28 +980,28 @@
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="30" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="30" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="32"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="9">
@@ -1049,7 +1013,7 @@
       <c r="E2" s="8">
         <v>9000000</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="20">
         <v>11500000</v>
       </c>
       <c r="G2" s="7">
@@ -1058,7 +1022,7 @@
       <c r="H2" s="8">
         <v>15000000</v>
       </c>
-      <c r="I2" s="36">
+      <c r="I2" s="20">
         <v>0</v>
       </c>
       <c r="J2" s="7">
@@ -1072,8 +1036,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2">
@@ -1085,7 +1049,7 @@
       <c r="E3" s="3">
         <v>9</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="21">
         <v>1</v>
       </c>
       <c r="G3" s="1">
@@ -1094,7 +1058,7 @@
       <c r="H3" s="3">
         <v>10</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="21">
         <v>6</v>
       </c>
       <c r="J3" s="1">
@@ -1108,8 +1072,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -1118,19 +1082,19 @@
       <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="24" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="22" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="10" t="s">
@@ -1143,81 +1107,81 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="41">
-        <f xml:space="preserve"> (0.3 * C2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (C3/2) * 12))</f>
-        <v>53682.340983749811</v>
-      </c>
-      <c r="D5" s="19">
-        <f xml:space="preserve"> (0.6 * D2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (D3/2) * 12))</f>
-        <v>119962.63940144314</v>
-      </c>
-      <c r="E5" s="42">
-        <f xml:space="preserve"> (0.6 * E2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (E3/2) * 12))</f>
-        <v>102825.11948695125</v>
-      </c>
-      <c r="F5" s="44">
-        <f xml:space="preserve"> (0.3 * F2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (F3/2) * 12))</f>
-        <v>405710.98362278962</v>
-      </c>
-      <c r="G5" s="19">
-        <f xml:space="preserve"> (G2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (G3/2) * 12))</f>
-        <v>214729.36393499924</v>
-      </c>
-      <c r="H5" s="42">
-        <f xml:space="preserve"> (H2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (H3/2) * 12))</f>
-        <v>268411.70491874905</v>
-      </c>
-      <c r="I5" s="28" t="s">
+      <c r="C5" s="25">
+        <f xml:space="preserve"> (0.3 * C2 * C3 * 0.0115) / (1 - (1 + 0.0115)^(-1 * (C3/2) * 12))</f>
+        <v>694940.80508991017</v>
+      </c>
+      <c r="D5" s="25">
+        <f t="shared" ref="D5:H5" si="0" xml:space="preserve"> (0.3 * D2 * D3 * 0.0115) / (1 - (1 + 0.0115)^(-1 * (D3/2) * 12))</f>
+        <v>707695.37880214816</v>
+      </c>
+      <c r="E5" s="25">
+        <f t="shared" si="0"/>
+        <v>606596.03897326987</v>
+      </c>
+      <c r="F5" s="25">
+        <f t="shared" si="0"/>
+        <v>598364.26086927566</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="0"/>
+        <v>833928.96610789222</v>
+      </c>
+      <c r="H5" s="25">
+        <f t="shared" si="0"/>
+        <v>1042411.2076348653</v>
+      </c>
+      <c r="I5" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="32" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="17">
-        <f xml:space="preserve"> (0.7 * C2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (C3/2) * 12))</f>
-        <v>125258.79562874956</v>
-      </c>
-      <c r="D6" s="18">
-        <f xml:space="preserve"> (0.4 * D2 * 0.0099) / (1 - (1 + 0.0099)^(-1.5 * (D3/2) * 12))</f>
-        <v>75634.112581131703</v>
-      </c>
-      <c r="E6" s="46">
-        <f xml:space="preserve"> (0.4 * E2 * 0.0099) / (1 - (1 + 0.0099)^(-1.5 * (E3/2) * 12))</f>
-        <v>64829.239355255741</v>
-      </c>
-      <c r="F6" s="45">
-        <f xml:space="preserve"> (0.7 * F2 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (F3/2) * 12))</f>
-        <v>946658.96178650903</v>
-      </c>
-      <c r="G6" s="43" t="s">
+      <c r="C6" s="25">
+        <f xml:space="preserve"> (0.3 * C2 * C3 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (C3/2) * 12))</f>
+        <v>536823.4098374981</v>
+      </c>
+      <c r="D6" s="25">
+        <f t="shared" ref="D6:F6" si="1" xml:space="preserve"> (0.3 * D2 * D3 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (D3/2) * 12))</f>
+        <v>539831.87730649416</v>
+      </c>
+      <c r="E6" s="25">
+        <f t="shared" si="1"/>
+        <v>462713.03769128065</v>
+      </c>
+      <c r="F6" s="25">
+        <f t="shared" si="1"/>
+        <v>405710.98362278962</v>
+      </c>
+      <c r="G6" s="26" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="23"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="33"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
@@ -1227,15 +1191,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
all test implemented and exceptions module
</commit_message>
<xml_diff>
--- a/Casos de Prueba.xlsx
+++ b/Casos de Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinil\Desktop\Universidad\Semestre 3\Codigo Limpio\Proyecto de aula\Icetex_Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508584DD-AA0F-45F6-82C9-545210C58C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27462CC-4716-48DB-A680-42FE2E5E4D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,14 +89,14 @@
     <t>Salidas</t>
   </si>
   <si>
-    <t>ERROR: La cantidad de semestres debe ser menor o igual a 10</t>
+    <t>ERROR: La cantidad de semestres debe ser un numero entero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +119,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -568,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -683,6 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +986,7 @@
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
       <c r="C1" s="27" t="s">
@@ -997,7 +1006,7 @@
       <c r="K1" s="28"/>
       <c r="L1" s="29"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>6</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>24000000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="18" t="s">
         <v>4</v>
@@ -1065,13 +1074,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="1">
-        <v>11</v>
+        <v>11.4</v>
       </c>
       <c r="L3" s="3">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
       <c r="B4" s="19" t="s">
         <v>5</v>
@@ -1107,7 +1116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>16</v>
       </c>
@@ -1127,8 +1136,8 @@
         <v>4840984.0933885006</v>
       </c>
       <c r="F5" s="25">
-        <f xml:space="preserve"> (0.3 * F2 * F3 * 0.0115) / (1 - (1 + 0.099)^(-1 * (F3/2) * 12))</f>
-        <v>91747.404601998263</v>
+        <f xml:space="preserve"> (0.3 * F2 * F3 * 0.0115) / (1 - (1 + 0.0115)^(-1 * (F3/2) * 12))</f>
+        <v>598364.26086927566</v>
       </c>
       <c r="G5" s="25">
         <f xml:space="preserve"> (G2 * G3 * 0.099) / (1 - (1 + 0.099)^(-1 * (G3/2) * 12))</f>
@@ -1151,7 +1160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37"/>
       <c r="B6" s="16" t="s">
         <v>10</v>
@@ -1169,8 +1178,8 @@
         <v>3209133.1146924561</v>
       </c>
       <c r="F6" s="25">
-        <f xml:space="preserve"> (0.3 * F2 * F3 * 0.0115) / (1 - (1 + 0.099)^(-1.5 * (F3/2) * 12))</f>
-        <v>69311.398989189736</v>
+        <f xml:space="preserve"> (0.7 * F2 * F3 * 0.0115) / (1 - (1 + 0.0115)^(-1.5 * (F3/2) * 12))</f>
+        <v>946658.96178650903</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>12</v>
@@ -1183,10 +1192,13 @@
       <c r="K6" s="31"/>
       <c r="L6" s="33"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="40"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D15" s="14"/>
     </row>
   </sheetData>

</xml_diff>